<commit_message>
Move data_analysis.py to archive for deprecation
</commit_message>
<xml_diff>
--- a/coin_data_template.xlsx
+++ b/coin_data_template.xlsx
@@ -466,12 +466,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>118408.05468750</t>
+          <t>118160.72656250</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>65547882496.00</t>
+          <t>66674782208.00</t>
         </is>
       </c>
     </row>
@@ -483,12 +483,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3600.63256836</t>
+          <t>3588.97875977</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>38585769984.00</t>
+          <t>40932126720.00</t>
         </is>
       </c>
     </row>
@@ -500,12 +500,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.23533821</t>
+          <t>3.13351941</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10529902592.00</t>
+          <t>12542594048.00</t>
         </is>
       </c>
     </row>
@@ -517,12 +517,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.00043166</t>
+          <t>1.00025249</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>135862927360.00</t>
+          <t>141775290368.00</t>
         </is>
       </c>
     </row>
@@ -534,12 +534,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>774.38476562</t>
+          <t>768.93322754</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3932507136.00</t>
+          <t>4054797312.00</t>
         </is>
       </c>
     </row>
@@ -551,12 +551,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>189.22950745</t>
+          <t>187.98310852</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>10183015424.00</t>
+          <t>10916662272.00</t>
         </is>
       </c>
     </row>
@@ -568,12 +568,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.00003898</t>
+          <t>0.99984008</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>15439869952.00</t>
+          <t>16324828160.00</t>
         </is>
       </c>
     </row>
@@ -585,12 +585,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.24357739</t>
+          <t>0.23768300</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3997614848.00</t>
+          <t>4269110016.00</t>
         </is>
       </c>
     </row>
@@ -602,12 +602,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.30987215</t>
+          <t>0.30729109</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1493277184.00</t>
+          <t>1655781120.00</t>
         </is>
       </c>
     </row>
@@ -619,12 +619,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3597.43652344</t>
+          <t>3570.79296875</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>149927840.00</t>
+          <t>148800512.00</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.81894785</t>
+          <t>0.80646747</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1736864512.00</t>
+          <t>1937128576.00</t>
         </is>
       </c>
     </row>
@@ -653,12 +653,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>118241.81250000</t>
+          <t>117959.80468750</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>331517536.00</t>
+          <t>353885984.00</t>
         </is>
       </c>
     </row>
@@ -670,12 +670,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.42815983</t>
+          <t>0.42064092</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>811856128.00</t>
+          <t>909483776.00</t>
         </is>
       </c>
     </row>
@@ -687,12 +687,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4341.61181641</t>
+          <t>4301.75244141</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14230802.00</t>
+          <t>15628827.00</t>
         </is>
       </c>
     </row>
@@ -704,12 +704,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>18.06451416</t>
+          <t>17.99403381</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>872778176.00</t>
+          <t>920663808.00</t>
         </is>
       </c>
     </row>
@@ -721,12 +721,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.24909009</t>
+          <t>0.24416417</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>640873728.00</t>
+          <t>703790464.00</t>
         </is>
       </c>
     </row>
@@ -738,12 +738,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>514.33441162</t>
+          <t>508.21533203</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>553494976.00</t>
+          <t>551133632.00</t>
         </is>
       </c>
     </row>
@@ -755,12 +755,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>23.92530060</t>
+          <t>23.71721458</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>890940608.00</t>
+          <t>906682688.00</t>
         </is>
       </c>
     </row>
@@ -772,12 +772,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>8.96855259</t>
+          <t>8.96154785</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>4274984.00</t>
+          <t>4582737.00</t>
         </is>
       </c>
     </row>
@@ -789,12 +789,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3851.85302734</t>
+          <t>3808.16894531</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>12030282.00</t>
+          <t>8637443.00</t>
         </is>
       </c>
     </row>
@@ -806,12 +806,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.00001400</t>
+          <t>0.00001374</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>436181952.00</t>
+          <t>475206848.00</t>
         </is>
       </c>
     </row>
@@ -823,12 +823,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.23924184</t>
+          <t>1.20425153</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>381588.00</t>
+          <t>336287.00</t>
         </is>
       </c>
     </row>
@@ -840,12 +840,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3603.57983398</t>
+          <t>3583.41235352</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1694144640.00</t>
+          <t>1783080704.00</t>
         </is>
       </c>
     </row>
@@ -857,12 +857,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>112.99745178</t>
+          <t>111.48131561</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1270145920.00</t>
+          <t>1322818048.00</t>
         </is>
       </c>
     </row>
@@ -874,12 +874,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>43.93137741</t>
+          <t>43.87120819</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>75550016.00</t>
+          <t>76108504.00</t>
         </is>
       </c>
     </row>
@@ -891,12 +891,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>317.05545044</t>
+          <t>311.20404053</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>118859808.00</t>
+          <t>117212760.00</t>
         </is>
       </c>
     </row>
@@ -908,12 +908,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4.15816307</t>
+          <t>4.09795761</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>506219904.00</t>
+          <t>533417792.00</t>
         </is>
       </c>
     </row>
@@ -925,12 +925,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4.67217588</t>
+          <t>4.66845989</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>189614512.00</t>
+          <t>196493424.00</t>
         </is>
       </c>
     </row>
@@ -942,12 +942,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>290.96365356</t>
+          <t>288.29605103</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>646104576.00</t>
+          <t>659059776.00</t>
         </is>
       </c>
     </row>
@@ -959,12 +959,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.99993175</t>
+          <t>0.99998087</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>23152211968.00</t>
+          <t>22987296768.00</t>
         </is>
       </c>
     </row>
@@ -976,12 +976,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.11997196</t>
+          <t>0.12048248</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>41141516.00</t>
+          <t>44030604.00</t>
         </is>
       </c>
     </row>
@@ -993,12 +993,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.08853078</t>
+          <t>1.07969487</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>135601968.00</t>
+          <t>145419184.00</t>
         </is>
       </c>
     </row>
@@ -1010,12 +1010,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.18515670</t>
+          <t>1.18500257</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>11617661.00</t>
+          <t>15223631.00</t>
         </is>
       </c>
     </row>
@@ -1027,12 +1027,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2.76159358</t>
+          <t>2.74254537</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>305102208.00</t>
+          <t>317335040.00</t>
         </is>
       </c>
     </row>
@@ -1044,12 +1044,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.02774727</t>
+          <t>1.01767731</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>500577888.00</t>
+          <t>492531552.00</t>
         </is>
       </c>
     </row>
@@ -1061,12 +1061,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>5.60961819</t>
+          <t>5.54796457</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>126178560.00</t>
+          <t>133150904.00</t>
         </is>
       </c>
     </row>
@@ -1078,12 +1078,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>48.76440048</t>
+          <t>48.34008026</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>22809228.00</t>
+          <t>23989712.00</t>
         </is>
       </c>
     </row>
@@ -1095,12 +1095,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>230.80123901</t>
+          <t>228.97001648</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>52448108.00</t>
+          <t>56821368.00</t>
         </is>
       </c>
     </row>
@@ -1112,12 +1112,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>22.50278282</t>
+          <t>22.39555931</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>304752544.00</t>
+          <t>320569088.00</t>
         </is>
       </c>
     </row>
@@ -1129,12 +1129,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0.26851952</t>
+          <t>0.26463071</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>155571216.00</t>
+          <t>175466688.00</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.10507347</t>
+          <t>0.10362400</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>134358400.00</t>
+          <t>141669360.00</t>
         </is>
       </c>
     </row>
@@ -1163,12 +1163,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.00003256</t>
+          <t>0.00003419</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1158361600.00</t>
+          <t>1302272896.00</t>
         </is>
       </c>
     </row>
@@ -1180,12 +1180,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.46665201</t>
+          <t>0.45273060</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>651786496.00</t>
+          <t>680827200.00</t>
         </is>
       </c>
     </row>
@@ -1197,12 +1197,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.02553111</t>
+          <t>0.02533145</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>77753888.00</t>
+          <t>84411136.00</t>
         </is>
       </c>
     </row>
@@ -1214,12 +1214,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>4.73022413</t>
+          <t>4.67824030</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>186956624.00</t>
+          <t>202652816.00</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1248,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.33050498</t>
+          <t>0.32917556</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>264532208.00</t>
+          <t>286890944.00</t>
         </is>
       </c>
     </row>
@@ -1265,12 +1265,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>4.50681496</t>
+          <t>4.51130533</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>64147348.00</t>
+          <t>62996956.00</t>
         </is>
       </c>
     </row>
@@ -1282,12 +1282,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>4.19209385</t>
+          <t>4.13666630</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>122344352.00</t>
+          <t>132999544.00</t>
         </is>
       </c>
     </row>
@@ -1299,12 +1299,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>17.71272469</t>
+          <t>17.47446251</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>16886856.00</t>
+          <t>16744707.00</t>
         </is>
       </c>
     </row>
@@ -1333,12 +1333,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.74180347</t>
+          <t>0.73909938</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>194440912.00</t>
+          <t>204704160.00</t>
         </is>
       </c>
     </row>
@@ -1350,12 +1350,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.19821894</t>
+          <t>1.16557431</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>705740160.00</t>
+          <t>645574208.00</t>
         </is>
       </c>
     </row>
@@ -1367,12 +1367,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2.66145182</t>
+          <t>2.62217665</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>317161408.00</t>
+          <t>340565664.00</t>
         </is>
       </c>
     </row>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.05327058</t>
+          <t>0.05325356</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1401,12 +1401,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>121.33161163</t>
+          <t>119.74081421</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>42022612.00</t>
+          <t>42349740.00</t>
         </is>
       </c>
     </row>
@@ -1418,12 +1418,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>201.20835876</t>
+          <t>199.69749451</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>7644157.00</t>
+          <t>7733124.00</t>
         </is>
       </c>
     </row>
@@ -1435,12 +1435,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5.09122467</t>
+          <t>5.07606983</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>31673888.00</t>
+          <t>33839248.00</t>
         </is>
       </c>
     </row>
@@ -1452,12 +1452,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.00098735</t>
+          <t>0.00098251</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>732.00</t>
+          <t>352.00</t>
         </is>
       </c>
     </row>
@@ -1469,12 +1469,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12.07556438</t>
+          <t>12.06196022</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>5338173.00</t>
+          <t>6182543.00</t>
         </is>
       </c>
     </row>
@@ -1486,12 +1486,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.99807614</t>
+          <t>0.99814290</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>9888662528.00</t>
+          <t>10459112448.00</t>
         </is>
       </c>
     </row>
@@ -1503,12 +1503,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>3779.37060547</t>
+          <t>3750.54223633</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>108860.00</t>
+          <t>555469.00</t>
         </is>
       </c>
     </row>
@@ -1520,12 +1520,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4103.11669922</t>
+          <t>4058.71826172</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>8190713.00</t>
+          <t>4752222.00</t>
         </is>
       </c>
     </row>
@@ -1537,12 +1537,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.97645199</t>
+          <t>1.92223394</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>174250960.00</t>
+          <t>187665760.00</t>
         </is>
       </c>
     </row>
@@ -1554,12 +1554,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.32596076</t>
+          <t>1.31564105</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>14370968.00</t>
+          <t>14184971.00</t>
         </is>
       </c>
     </row>
@@ -1571,12 +1571,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4.93759823</t>
+          <t>4.97862434</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>33274076.00</t>
+          <t>33674876.00</t>
         </is>
       </c>
     </row>
@@ -1588,12 +1588,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.54248261</t>
+          <t>1.51207006</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>387730592.00</t>
+          <t>390288192.00</t>
         </is>
       </c>
     </row>
@@ -1605,12 +1605,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>13.86128235</t>
+          <t>13.73220444</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>169027808.00</t>
+          <t>175816432.00</t>
         </is>
       </c>
     </row>
@@ -1622,12 +1622,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0.00001286</t>
+          <t>0.00001261</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1412940800.00</t>
+          <t>1492878592.00</t>
         </is>
       </c>
     </row>
@@ -1639,12 +1639,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.02320885</t>
+          <t>0.02286448</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>98168264.00</t>
+          <t>97335344.00</t>
         </is>
       </c>
     </row>
@@ -1656,12 +1656,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.08774082</t>
+          <t>0.08519785</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>55723684.00</t>
+          <t>58277992.00</t>
         </is>
       </c>
     </row>
@@ -1673,12 +1673,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.70646709</t>
+          <t>0.68822592</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>308356736.00</t>
+          <t>330961632.00</t>
         </is>
       </c>
     </row>
@@ -1690,12 +1690,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3785.68725586</t>
+          <t>3747.10180664</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>39548.00</t>
+          <t>40637.00</t>
         </is>
       </c>
     </row>
@@ -1707,12 +1707,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>118139.06250000</t>
+          <t>117959.69531250</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1321481.00</t>
+          <t>1401545.00</t>
         </is>
       </c>
     </row>
@@ -1724,12 +1724,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.73458755</t>
+          <t>1.68242478</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>309425568.00</t>
+          <t>323265184.00</t>
         </is>
       </c>
     </row>
@@ -1741,12 +1741,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0.80413878</t>
+          <t>0.79622054</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>286088224.00</t>
+          <t>370313824.00</t>
         </is>
       </c>
     </row>

</xml_diff>